<commit_message>
added NSDL Test Automation.
</commit_message>
<xml_diff>
--- a/KYC/QA/PrimeBankKYC/data/KYC_Poc.xlsx
+++ b/KYC/QA/PrimeBankKYC/data/KYC_Poc.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{34FE9C13-8BA7-4296-BE55-E589BB68C87C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F55157-E2C7-4400-9C60-2DBF2DF837A7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="KYC_Home_Login_Screen" r:id="rId1" sheetId="1"/>
-    <sheet name="KYC_RegistrationPage" r:id="rId2" sheetId="2"/>
+    <sheet name="KYC_Home_Login_Screen" sheetId="1" r:id="rId1"/>
+    <sheet name="KYC_RegistrationPage" sheetId="2" r:id="rId2"/>
+    <sheet name="NSDL_Login_Page" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021" calcMode="manual"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="268">
   <si>
     <t>UserName</t>
   </si>
@@ -795,13 +796,42 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>NSDL_Login_ValidUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_InvalidUserName</t>
+  </si>
+  <si>
+    <t>NSDL_Login_ValidUserName_InvalidPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_BlankUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_ValidUserName_BlankPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_BlankUserName_BlankPwd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -852,38 +882,41 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="16" xfId="0">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -900,10 +933,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -938,7 +971,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -973,7 +1006,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1067,21 +1100,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1098,7 +1131,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1150,27 +1183,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="43.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
-    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="43" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1190,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1236,7 +1269,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,36 +1316,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F60070-FAD4-4BB1-B9EA-BB1B58E5D3F9}">
-  <dimension ref="A1:X33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F60070-FAD4-4BB1-B9EA-BB1B58E5D3F9}">
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="6" width="51.28515625" collapsed="true"/>
-    <col min="2" max="6" style="6" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="7" width="18.28515625" collapsed="true"/>
-    <col min="8" max="9" style="6" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="6" width="14.7109375" collapsed="true"/>
-    <col min="11" max="17" style="6" width="9.140625" collapsed="true"/>
-    <col min="18" max="18" style="7" width="9.140625" collapsed="true"/>
-    <col min="19" max="19" style="6" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="7" width="11.0" collapsed="true"/>
-    <col min="21" max="21" style="6" width="9.140625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="6" width="18.140625" collapsed="true"/>
-    <col min="23" max="16384" style="6" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="51.28515625" style="6" customWidth="1" collapsed="1"/>
+    <col min="2" max="6" width="9.140625" style="6" collapsed="1"/>
+    <col min="7" max="7" width="18.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="6" collapsed="1"/>
+    <col min="9" max="9" width="22.28515625" style="6" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.7109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="6" collapsed="1"/>
+    <col min="12" max="12" width="20.85546875" style="6" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="9.140625" style="6" collapsed="1"/>
+    <col min="18" max="18" width="9.140625" style="7" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="6" collapsed="1"/>
+    <col min="20" max="20" width="11" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="9.140625" style="6" collapsed="1"/>
+    <col min="22" max="22" width="18.140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="23" max="16384" width="9.140625" style="6" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="45" r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1383,14 +1419,14 @@
         <v>6</v>
       </c>
     </row>
-    <row ht="60" r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1445,12 +1481,12 @@
       <c r="U2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="V2"/>
-      <c r="W2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="60" r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V2" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W2" s="4"/>
+    </row>
+    <row r="3" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>52</v>
       </c>
@@ -1460,7 +1496,7 @@
       <c r="C3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1477,13 +1513,13 @@
         <v>70</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="M3" s="1">
         <v>102</v>
@@ -1512,12 +1548,12 @@
       <c r="U3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="V3"/>
-      <c r="W3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V3" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W3" s="4"/>
+    </row>
+    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
@@ -1530,7 +1566,7 @@
       <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1" t="s">
         <v>81</v>
       </c>
@@ -1579,12 +1615,12 @@
       <c r="U4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="V4"/>
-      <c r="W4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="75" r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V4" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W4" s="4"/>
+    </row>
+    <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>54</v>
       </c>
@@ -1600,7 +1636,7 @@
       <c r="E5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F5"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="2">
         <v>952615274529</v>
       </c>
@@ -1608,7 +1644,7 @@
         <v>94</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>96</v>
@@ -1646,12 +1682,12 @@
       <c r="U5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="V5"/>
-      <c r="W5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="75" r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V5" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>55</v>
       </c>
@@ -1670,12 +1706,12 @@
       <c r="F6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G6"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="1" t="s">
         <v>105</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>107</v>
@@ -1713,12 +1749,12 @@
       <c r="U6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="V6"/>
-      <c r="W6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V6" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W6" s="4"/>
+    </row>
+    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
@@ -1740,7 +1776,7 @@
       <c r="G7" s="2">
         <v>985796482456</v>
       </c>
-      <c r="H7"/>
+      <c r="H7" s="4"/>
       <c r="I7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1751,7 +1787,7 @@
         <v>118</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="M7" s="1">
         <v>109</v>
@@ -1780,12 +1816,12 @@
       <c r="U7" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="V7"/>
-      <c r="W7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V7" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W7" s="4"/>
+    </row>
+    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
@@ -1798,7 +1834,9 @@
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E8"/>
+      <c r="E8" s="9" t="s">
+        <v>258</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>125</v>
       </c>
@@ -1808,9 +1846,11 @@
       <c r="H8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I8"/>
+      <c r="I8" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>128</v>
@@ -1845,12 +1885,12 @@
       <c r="U8" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="V8"/>
-      <c r="W8" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V8" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W8" s="4"/>
+    </row>
+    <row r="9" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -1878,7 +1918,9 @@
       <c r="I9" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J9"/>
+      <c r="J9" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="K9" s="1" t="s">
         <v>138</v>
       </c>
@@ -1912,12 +1954,12 @@
       <c r="U9" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="V9"/>
-      <c r="W9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="30" r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W9" s="4"/>
+    </row>
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>214</v>
       </c>
@@ -1948,7 +1990,9 @@
       <c r="J10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K10"/>
+      <c r="K10" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="L10" s="1" t="s">
         <v>43</v>
       </c>
@@ -1979,12 +2023,12 @@
       <c r="U10" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="V10"/>
-      <c r="W10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="60" r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V10" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W10" s="4"/>
+    </row>
+    <row r="11" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>215</v>
       </c>
@@ -2018,7 +2062,9 @@
       <c r="K11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L11"/>
+      <c r="L11" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="M11" s="1">
         <v>294</v>
       </c>
@@ -2046,12 +2092,12 @@
       <c r="U11" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="V11"/>
-      <c r="W11" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V11" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W11" s="4"/>
+    </row>
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>218</v>
       </c>
@@ -2088,7 +2134,7 @@
       <c r="L12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M12"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="1" t="s">
         <v>167</v>
       </c>
@@ -2113,12 +2159,12 @@
       <c r="U12" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="V12"/>
-      <c r="W12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="75" r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V12" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>222</v>
       </c>
@@ -2144,7 +2190,7 @@
         <v>175</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>71</v>
@@ -2158,7 +2204,7 @@
       <c r="M13" s="1">
         <v>253</v>
       </c>
-      <c r="N13"/>
+      <c r="N13" s="4"/>
       <c r="O13" s="1" t="s">
         <v>176</v>
       </c>
@@ -2180,12 +2226,12 @@
       <c r="U13" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="V13"/>
-      <c r="W13" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="30" r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V13" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W13" s="4"/>
+    </row>
+    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>223</v>
       </c>
@@ -2228,7 +2274,7 @@
       <c r="N14" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="O14"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="1" t="s">
         <v>186</v>
       </c>
@@ -2247,12 +2293,12 @@
       <c r="U14" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="V14"/>
-      <c r="W14" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V14" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W14" s="4"/>
+    </row>
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>224</v>
       </c>
@@ -2298,7 +2344,7 @@
       <c r="O15" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="P15"/>
+      <c r="P15" s="4"/>
       <c r="Q15" s="1" t="s">
         <v>196</v>
       </c>
@@ -2314,12 +2360,12 @@
       <c r="U15" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="V15"/>
-      <c r="W15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V15" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W15" s="4"/>
+    </row>
+    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>225</v>
       </c>
@@ -2368,7 +2414,7 @@
       <c r="P16" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="Q16"/>
+      <c r="Q16" s="4"/>
       <c r="R16" s="1">
         <v>953157</v>
       </c>
@@ -2381,12 +2427,12 @@
       <c r="U16" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="V16"/>
-      <c r="W16" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="W16" s="4"/>
+    </row>
+    <row r="17" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>226</v>
       </c>
@@ -2438,7 +2484,7 @@
       <c r="Q17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="R17"/>
+      <c r="R17" s="4"/>
       <c r="S17" s="1" t="s">
         <v>49</v>
       </c>
@@ -2448,12 +2494,12 @@
       <c r="U17" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="V17"/>
-      <c r="W17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W17" s="4"/>
+    </row>
+    <row r="18" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>227</v>
       </c>
@@ -2508,19 +2554,19 @@
       <c r="R18" s="1">
         <v>975351</v>
       </c>
-      <c r="S18"/>
+      <c r="S18" s="4"/>
       <c r="T18" s="1">
         <v>9756842138</v>
       </c>
       <c r="U18" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="V18"/>
-      <c r="W18" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W18" s="4"/>
+    </row>
+    <row r="19" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>228</v>
       </c>
@@ -2578,16 +2624,16 @@
       <c r="S19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T19"/>
+      <c r="T19" s="4"/>
       <c r="U19" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="V19"/>
-      <c r="W19" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W19" s="4"/>
+    </row>
+    <row r="20" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>229</v>
       </c>
@@ -2648,13 +2694,13 @@
       <c r="T20" s="1">
         <v>9764851329</v>
       </c>
-      <c r="U20"/>
-      <c r="V20"/>
-      <c r="W20" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U20" s="4"/>
+      <c r="V20" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W20" s="4"/>
+    </row>
+    <row r="21" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>230</v>
       </c>
@@ -2718,12 +2764,12 @@
       <c r="U21" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="V21"/>
-      <c r="W21" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>232</v>
       </c>
@@ -2787,12 +2833,12 @@
       <c r="U22" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="V22"/>
-      <c r="W22" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W22" s="4"/>
+    </row>
+    <row r="23" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>243</v>
       </c>
@@ -2856,12 +2902,12 @@
       <c r="U23" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="V23"/>
-      <c r="W23" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W23" s="4"/>
+    </row>
+    <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>234</v>
       </c>
@@ -2919,16 +2965,16 @@
       <c r="S24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T24"/>
+      <c r="T24" s="4"/>
       <c r="U24" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="V24"/>
-      <c r="W24" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W24" s="4"/>
+    </row>
+    <row r="25" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>237</v>
       </c>
@@ -2983,19 +3029,19 @@
       <c r="R25" s="1">
         <v>975351</v>
       </c>
-      <c r="S25"/>
+      <c r="S25" s="4"/>
       <c r="T25" s="1">
         <v>9756842138</v>
       </c>
       <c r="U25" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="V25"/>
-      <c r="W25" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="75" r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W25" s="4"/>
+    </row>
+    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>239</v>
       </c>
@@ -3059,12 +3105,12 @@
       <c r="U26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="V26"/>
-      <c r="W26" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="60" r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W26" s="4"/>
+    </row>
+    <row r="27" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>241</v>
       </c>
@@ -3128,12 +3174,12 @@
       <c r="U27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="V27"/>
-      <c r="W27" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="60" r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W27" s="4"/>
+    </row>
+    <row r="28" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>242</v>
       </c>
@@ -3197,12 +3243,12 @@
       <c r="U28" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="V28"/>
-      <c r="W28" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W28" s="4"/>
+    </row>
+    <row r="29" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>245</v>
       </c>
@@ -3266,12 +3312,12 @@
       <c r="U29" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="V29"/>
-      <c r="W29" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W29" s="4"/>
+    </row>
+    <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>247</v>
       </c>
@@ -3335,12 +3381,12 @@
       <c r="U30" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="V30"/>
-      <c r="W30" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W30" s="4"/>
+    </row>
+    <row r="31" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>249</v>
       </c>
@@ -3404,12 +3450,12 @@
       <c r="U31" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="V31"/>
-      <c r="W31" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W31" s="4"/>
+    </row>
+    <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>250</v>
       </c>
@@ -3473,12 +3519,12 @@
       <c r="U32" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="V32"/>
-      <c r="W32" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row ht="45" r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W32" s="4"/>
+    </row>
+    <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>251</v>
       </c>
@@ -3542,46 +3588,160 @@
       <c r="U33" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="V33"/>
-      <c r="W33" t="s">
-        <v>257</v>
-      </c>
+      <c r="V33" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="W33" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="U2" xr:uid="{AD2E7342-13F3-4F9E-8E52-A4A5C93E59C5}"/>
-    <hyperlink r:id="rId2" ref="U3" xr:uid="{29E24696-ABE1-400D-9555-90AA7E0B37DB}"/>
-    <hyperlink r:id="rId3" ref="U4" xr:uid="{CCAF1C57-5CAA-46A4-9FDE-DC7CCCBA1FE2}"/>
-    <hyperlink r:id="rId4" ref="U5" xr:uid="{B3D432BD-5DC1-4DC7-8345-27CBF5E7A7B8}"/>
-    <hyperlink r:id="rId5" ref="U6" xr:uid="{3FDA59A3-9F97-476D-940E-F9F8F3419590}"/>
-    <hyperlink r:id="rId6" ref="U7" xr:uid="{EE21543B-4101-44AC-A791-BB020D67D15A}"/>
-    <hyperlink r:id="rId7" ref="U8" xr:uid="{32FDA270-E1F7-4995-8E37-B67AC9DD3235}"/>
-    <hyperlink r:id="rId8" ref="U9" xr:uid="{BF6141EC-4057-4024-874D-477765760585}"/>
-    <hyperlink r:id="rId9" ref="U10" xr:uid="{499AE279-0ED2-4CD7-8F13-139FE1A622CC}"/>
-    <hyperlink r:id="rId10" ref="U11" xr:uid="{3662C424-4C41-4250-B209-CDBACC7A71DA}"/>
-    <hyperlink r:id="rId11" ref="U12" xr:uid="{289EC856-9D51-4814-A650-D5A3B00ECC0C}"/>
-    <hyperlink r:id="rId12" ref="U13" xr:uid="{3457B279-724D-4979-BED6-2B8D01AC0924}"/>
-    <hyperlink r:id="rId13" ref="U14" xr:uid="{BE633FB0-EF01-48CB-8C71-635435699C5D}"/>
-    <hyperlink r:id="rId14" ref="U15" xr:uid="{5A83CB1D-4B01-46C3-8AE1-B39AA1430B94}"/>
-    <hyperlink r:id="rId15" ref="U16" xr:uid="{B14B822F-C21C-45A6-9F7E-B221B6998A4F}"/>
-    <hyperlink r:id="rId16" ref="U17" xr:uid="{17A344FC-B915-4271-BD66-3CE2516C36C9}"/>
-    <hyperlink r:id="rId17" ref="U18" xr:uid="{3F2C047A-5A19-46D7-AC7D-025B60279EC0}"/>
-    <hyperlink r:id="rId18" ref="U19" xr:uid="{9D0F7785-F305-41DD-9E52-2BE70A95E805}"/>
-    <hyperlink r:id="rId19" ref="U21" xr:uid="{87FE59FB-6A12-4CF9-A01C-E45985D7BEB9}"/>
-    <hyperlink r:id="rId20" ref="U22" xr:uid="{94815C58-70FB-4B56-9A95-4C6DF393AB8B}"/>
-    <hyperlink r:id="rId21" ref="U24" xr:uid="{0D5D67AA-0F64-4B48-B39E-51AE702FA16C}"/>
-    <hyperlink r:id="rId22" ref="U25" xr:uid="{96A0CE36-EDF9-4C31-9319-B656541D8E0C}"/>
-    <hyperlink r:id="rId23" ref="U26" xr:uid="{623CADAB-4274-4755-A141-B35BDB09B4B6}"/>
-    <hyperlink r:id="rId24" ref="U27" xr:uid="{B44FE402-C265-4AEF-9B14-D15BF35C1DBA}"/>
-    <hyperlink r:id="rId25" ref="U28" xr:uid="{6512C6AF-E70C-4FF2-9970-5C6D37EB2E59}"/>
-    <hyperlink r:id="rId26" ref="U23" xr:uid="{EFDCE50D-AE7D-4C63-BB97-0273A329B531}"/>
-    <hyperlink r:id="rId27" ref="U29" xr:uid="{5E27030D-F479-497D-9434-F5E7113CE60E}"/>
-    <hyperlink r:id="rId28" ref="U30" xr:uid="{B93A6E59-B895-40DD-BE44-873C07EC1794}"/>
-    <hyperlink r:id="rId29" ref="U31" xr:uid="{CC221388-8D4E-4326-ADBC-A8DF4471F271}"/>
-    <hyperlink r:id="rId30" ref="U32" xr:uid="{8D7E4050-6D3E-4A7F-A832-EDC7FD964D79}"/>
-    <hyperlink r:id="rId31" ref="U33" xr:uid="{CF689C5F-9073-4A89-8BDA-2602AD6EED14}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{AD2E7342-13F3-4F9E-8E52-A4A5C93E59C5}"/>
+    <hyperlink ref="U3" r:id="rId2" xr:uid="{29E24696-ABE1-400D-9555-90AA7E0B37DB}"/>
+    <hyperlink ref="U4" r:id="rId3" xr:uid="{CCAF1C57-5CAA-46A4-9FDE-DC7CCCBA1FE2}"/>
+    <hyperlink ref="U5" r:id="rId4" xr:uid="{B3D432BD-5DC1-4DC7-8345-27CBF5E7A7B8}"/>
+    <hyperlink ref="U6" r:id="rId5" xr:uid="{3FDA59A3-9F97-476D-940E-F9F8F3419590}"/>
+    <hyperlink ref="U7" r:id="rId6" xr:uid="{EE21543B-4101-44AC-A791-BB020D67D15A}"/>
+    <hyperlink ref="U8" r:id="rId7" xr:uid="{32FDA270-E1F7-4995-8E37-B67AC9DD3235}"/>
+    <hyperlink ref="U9" r:id="rId8" xr:uid="{BF6141EC-4057-4024-874D-477765760585}"/>
+    <hyperlink ref="U10" r:id="rId9" xr:uid="{499AE279-0ED2-4CD7-8F13-139FE1A622CC}"/>
+    <hyperlink ref="U11" r:id="rId10" xr:uid="{3662C424-4C41-4250-B209-CDBACC7A71DA}"/>
+    <hyperlink ref="U12" r:id="rId11" xr:uid="{289EC856-9D51-4814-A650-D5A3B00ECC0C}"/>
+    <hyperlink ref="U13" r:id="rId12" xr:uid="{3457B279-724D-4979-BED6-2B8D01AC0924}"/>
+    <hyperlink ref="U14" r:id="rId13" xr:uid="{BE633FB0-EF01-48CB-8C71-635435699C5D}"/>
+    <hyperlink ref="U15" r:id="rId14" xr:uid="{5A83CB1D-4B01-46C3-8AE1-B39AA1430B94}"/>
+    <hyperlink ref="U16" r:id="rId15" xr:uid="{B14B822F-C21C-45A6-9F7E-B221B6998A4F}"/>
+    <hyperlink ref="U17" r:id="rId16" xr:uid="{17A344FC-B915-4271-BD66-3CE2516C36C9}"/>
+    <hyperlink ref="U18" r:id="rId17" xr:uid="{3F2C047A-5A19-46D7-AC7D-025B60279EC0}"/>
+    <hyperlink ref="U19" r:id="rId18" xr:uid="{9D0F7785-F305-41DD-9E52-2BE70A95E805}"/>
+    <hyperlink ref="U21" r:id="rId19" xr:uid="{87FE59FB-6A12-4CF9-A01C-E45985D7BEB9}"/>
+    <hyperlink ref="U22" r:id="rId20" xr:uid="{94815C58-70FB-4B56-9A95-4C6DF393AB8B}"/>
+    <hyperlink ref="U24" r:id="rId21" xr:uid="{0D5D67AA-0F64-4B48-B39E-51AE702FA16C}"/>
+    <hyperlink ref="U25" r:id="rId22" xr:uid="{96A0CE36-EDF9-4C31-9319-B656541D8E0C}"/>
+    <hyperlink ref="U26" r:id="rId23" xr:uid="{623CADAB-4274-4755-A141-B35BDB09B4B6}"/>
+    <hyperlink ref="U27" r:id="rId24" xr:uid="{B44FE402-C265-4AEF-9B14-D15BF35C1DBA}"/>
+    <hyperlink ref="U28" r:id="rId25" xr:uid="{6512C6AF-E70C-4FF2-9970-5C6D37EB2E59}"/>
+    <hyperlink ref="U23" r:id="rId26" xr:uid="{EFDCE50D-AE7D-4C63-BB97-0273A329B531}"/>
+    <hyperlink ref="U29" r:id="rId27" xr:uid="{5E27030D-F479-497D-9434-F5E7113CE60E}"/>
+    <hyperlink ref="U30" r:id="rId28" xr:uid="{B93A6E59-B895-40DD-BE44-873C07EC1794}"/>
+    <hyperlink ref="U31" r:id="rId29" xr:uid="{CC221388-8D4E-4326-ADBC-A8DF4471F271}"/>
+    <hyperlink ref="U32" r:id="rId30" xr:uid="{8D7E4050-6D3E-4A7F-A832-EDC7FD964D79}"/>
+    <hyperlink ref="U33" r:id="rId31" xr:uid="{CF689C5F-9073-4A89-8BDA-2602AD6EED14}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F6B53-E569-4B89-A652-F5C31A5C1A46}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added scripts for all cases.
</commit_message>
<xml_diff>
--- a/KYC/QA/PrimeBankKYC/data/KYC_Poc.xlsx
+++ b/KYC/QA/PrimeBankKYC/data/KYC_Poc.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F55157-E2C7-4400-9C60-2DBF2DF837A7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:801_{461342A1-4BD5-471E-A685-30FCC9F0EFA7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="2" firstSheet="2" windowHeight="8040" windowWidth="15030" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="KYC_Home_Login_Screen" sheetId="1" r:id="rId1"/>
-    <sheet name="KYC_RegistrationPage" sheetId="2" r:id="rId2"/>
-    <sheet name="NSDL_Login_Page" sheetId="3" r:id="rId3"/>
+    <sheet name="KYC_Home_Login_Screen" r:id="rId1" sheetId="1"/>
+    <sheet name="KYC_RegistrationPage" r:id="rId2" sheetId="2"/>
+    <sheet name="KYC_NSDL_Login_Page" r:id="rId3" sheetId="3"/>
+    <sheet name="KYC_Aadhar_Login_Page" r:id="rId4" sheetId="4"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="7"/>
+    <sheet name="KYC_Passport_Login_Page" r:id="rId6" sheetId="5"/>
+    <sheet name="KYC_Aadhar_Verification_Page" r:id="rId7" sheetId="6"/>
+    <sheet name="KYC_NSDL_Verification_Page" r:id="rId8" sheetId="8"/>
+    <sheet name="KYC_Passport_Verification_Page" r:id="rId9" sheetId="9"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="0" calcMode="manual"/>
+  <oleSize ref="B1:J24"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="298">
   <si>
     <t>UserName</t>
   </si>
@@ -795,43 +802,134 @@
     <t>PASS</t>
   </si>
   <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>NSDL_Login_ValidUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_InvalidUserName</t>
+  </si>
+  <si>
+    <t>NSDL_Login_ValidUserName_InvalidPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_BlankUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_ValidUserName_BlankPwd</t>
+  </si>
+  <si>
+    <t>NSDL_Login_BlankUserName_BlankPwd</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Raj</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>NSDL_Login_ValidUserName_ValidPwd</t>
-  </si>
-  <si>
-    <t>NSDL_Login_InvalidUserName</t>
-  </si>
-  <si>
-    <t>NSDL_Login_ValidUserName_InvalidPwd</t>
-  </si>
-  <si>
-    <t>NSDL_Login_BlankUserName_ValidPwd</t>
-  </si>
-  <si>
-    <t>NSDL_Login_ValidUserName_BlankPwd</t>
-  </si>
-  <si>
-    <t>NSDL_Login_BlankUserName_BlankPwd</t>
+    <t>Aadhar_Login_InvalidUserName</t>
+  </si>
+  <si>
+    <t>Aadhar_Login_ValidUserName_InvalidPwd</t>
+  </si>
+  <si>
+    <t>Aadhar_Login_BlankUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>Aadhar_Login_ValidUserName_BlankPwd</t>
+  </si>
+  <si>
+    <t>Aadhar_Login_BlankUserName_BlankPwd</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>yhjkl</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>manage</t>
+  </si>
+  <si>
+    <t>Passport_Login_ValidUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>Passport_Login_InvalidUserName</t>
+  </si>
+  <si>
+    <t>Passport_Login_ValidUserName_InvalidPwd</t>
+  </si>
+  <si>
+    <t>Passport_Login_BlankUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>Passport_Login_ValidUserName_BlankPwd</t>
+  </si>
+  <si>
+    <t>Passport_Login_BlankUserName_BlankPwd</t>
+  </si>
+  <si>
+    <t>valid_aadhar_id</t>
+  </si>
+  <si>
+    <t>blank_aadhar_id</t>
+  </si>
+  <si>
+    <t>invalid_aadhar_id</t>
+  </si>
+  <si>
+    <t>Aadharnumber</t>
+  </si>
+  <si>
+    <t>Aadhar_Login_ValidUserName_ValidPwd</t>
+  </si>
+  <si>
+    <t>valid_pan_id</t>
+  </si>
+  <si>
+    <t>blank_pan_id</t>
+  </si>
+  <si>
+    <t>invalid_pan_id</t>
+  </si>
+  <si>
+    <t>Pannumber</t>
+  </si>
+  <si>
+    <t>QWERTY78</t>
+  </si>
+  <si>
+    <t>valid_passport_number</t>
+  </si>
+  <si>
+    <t>blank_passport_number</t>
+  </si>
+  <si>
+    <t>invalid_passport_number</t>
+  </si>
+  <si>
+    <t>Passportnumber</t>
+  </si>
+  <si>
+    <t>HAI123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -857,7 +955,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -880,43 +978,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="16" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -933,10 +1064,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -971,7 +1102,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1006,7 +1137,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1100,21 +1231,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1131,7 +1262,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1183,27 +1314,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="43.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
+    <col min="5" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1223,7 +1352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1237,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,7 +1381,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,7 +1398,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1284,7 +1413,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1299,7 +1428,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,43 +1441,43 @@
         <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F60070-FAD4-4BB1-B9EA-BB1B58E5D3F9}">
-  <dimension ref="A1:W33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F60070-FAD4-4BB1-B9EA-BB1B58E5D3F9}">
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" style="6" customWidth="1" collapsed="1"/>
-    <col min="2" max="6" width="9.140625" style="6" collapsed="1"/>
-    <col min="7" max="7" width="18.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="6" collapsed="1"/>
-    <col min="9" max="9" width="22.28515625" style="6" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.7109375" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.140625" style="6" collapsed="1"/>
-    <col min="12" max="12" width="20.85546875" style="6" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="9.140625" style="6" collapsed="1"/>
-    <col min="18" max="18" width="9.140625" style="7" collapsed="1"/>
-    <col min="19" max="19" width="9.140625" style="6" collapsed="1"/>
-    <col min="20" max="20" width="11" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.140625" style="6" collapsed="1"/>
-    <col min="22" max="22" width="18.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="23" max="16384" width="9.140625" style="6" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="6" width="51.28515625" collapsed="true"/>
+    <col min="2" max="6" style="6" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="7" width="18.28515625" collapsed="true"/>
+    <col min="8" max="8" style="6" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="6" width="22.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="14.7109375" collapsed="true"/>
+    <col min="11" max="11" style="6" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="6" width="20.85546875" collapsed="true"/>
+    <col min="13" max="17" style="6" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" style="7" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" style="6" width="9.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="7" width="11.0" collapsed="true"/>
+    <col min="21" max="21" style="6" width="9.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="6" width="18.140625" collapsed="true"/>
+    <col min="23" max="16384" style="6" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1419,14 +1548,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2"/>
       <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1482,11 +1611,13 @@
         <v>50</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="60" r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>52</v>
       </c>
@@ -1496,7 +1627,7 @@
       <c r="C3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3"/>
       <c r="E3" s="1" t="s">
         <v>67</v>
       </c>
@@ -1549,11 +1680,13 @@
         <v>78</v>
       </c>
       <c r="V3" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
@@ -1566,7 +1699,7 @@
       <c r="D4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4"/>
       <c r="F4" s="1" t="s">
         <v>81</v>
       </c>
@@ -1616,11 +1749,13 @@
         <v>91</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W4" s="4"/>
-    </row>
-    <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>54</v>
       </c>
@@ -1636,7 +1771,7 @@
       <c r="E5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5"/>
       <c r="G5" s="2">
         <v>952615274529</v>
       </c>
@@ -1683,11 +1818,13 @@
         <v>103</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W5" s="4"/>
-    </row>
-    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="30" r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>55</v>
       </c>
@@ -1706,7 +1843,7 @@
       <c r="F6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6"/>
       <c r="H6" s="1" t="s">
         <v>105</v>
       </c>
@@ -1750,11 +1887,13 @@
         <v>113</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W6" s="4"/>
-    </row>
-    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
@@ -1776,7 +1915,7 @@
       <c r="G7" s="2">
         <v>985796482456</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7"/>
       <c r="I7" s="1" t="s">
         <v>107</v>
       </c>
@@ -1817,11 +1956,13 @@
         <v>123</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W7" s="4"/>
-    </row>
-    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
@@ -1835,7 +1976,7 @@
         <v>36</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>125</v>
@@ -1847,7 +1988,7 @@
         <v>126</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>96</v>
@@ -1886,11 +2027,13 @@
         <v>133</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W8" s="4"/>
-    </row>
-    <row r="9" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -1919,7 +2062,7 @@
         <v>107</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>138</v>
@@ -1955,11 +2098,13 @@
         <v>143</v>
       </c>
       <c r="V9" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W9" s="4"/>
-    </row>
-    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="30" r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>214</v>
       </c>
@@ -1991,7 +2136,7 @@
         <v>96</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>43</v>
@@ -2024,11 +2169,13 @@
         <v>152</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W10" s="4"/>
-    </row>
-    <row r="11" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="60" r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>215</v>
       </c>
@@ -2063,7 +2210,7 @@
         <v>72</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M11" s="1">
         <v>294</v>
@@ -2093,11 +2240,13 @@
         <v>161</v>
       </c>
       <c r="V11" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W11" s="4"/>
-    </row>
-    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>218</v>
       </c>
@@ -2134,7 +2283,7 @@
       <c r="L12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12"/>
       <c r="N12" s="1" t="s">
         <v>167</v>
       </c>
@@ -2160,11 +2309,13 @@
         <v>171</v>
       </c>
       <c r="V12" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W12" s="4"/>
-    </row>
-    <row r="13" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>222</v>
       </c>
@@ -2204,7 +2355,7 @@
       <c r="M13" s="1">
         <v>253</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13"/>
       <c r="O13" s="1" t="s">
         <v>176</v>
       </c>
@@ -2227,11 +2378,13 @@
         <v>179</v>
       </c>
       <c r="V13" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W13" s="4"/>
-    </row>
-    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="30" r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>223</v>
       </c>
@@ -2274,7 +2427,7 @@
       <c r="N14" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="O14" s="4"/>
+      <c r="O14"/>
       <c r="P14" s="1" t="s">
         <v>186</v>
       </c>
@@ -2294,11 +2447,13 @@
         <v>188</v>
       </c>
       <c r="V14" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W14" s="4"/>
-    </row>
-    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>224</v>
       </c>
@@ -2344,7 +2499,7 @@
       <c r="O15" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="P15" s="4"/>
+      <c r="P15"/>
       <c r="Q15" s="1" t="s">
         <v>196</v>
       </c>
@@ -2361,11 +2516,13 @@
         <v>197</v>
       </c>
       <c r="V15" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W15" s="4"/>
-    </row>
-    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>225</v>
       </c>
@@ -2414,7 +2571,7 @@
       <c r="P16" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="Q16" s="4"/>
+      <c r="Q16"/>
       <c r="R16" s="1">
         <v>953157</v>
       </c>
@@ -2428,11 +2585,13 @@
         <v>205</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="W16" s="4"/>
-    </row>
-    <row r="17" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>226</v>
       </c>
@@ -2484,7 +2643,7 @@
       <c r="Q17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="R17" s="4"/>
+      <c r="R17"/>
       <c r="S17" s="1" t="s">
         <v>49</v>
       </c>
@@ -2495,11 +2654,13 @@
         <v>213</v>
       </c>
       <c r="V17" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W17" s="4"/>
-    </row>
-    <row r="18" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>227</v>
       </c>
@@ -2554,7 +2715,7 @@
       <c r="R18" s="1">
         <v>975351</v>
       </c>
-      <c r="S18" s="4"/>
+      <c r="S18"/>
       <c r="T18" s="1">
         <v>9756842138</v>
       </c>
@@ -2562,11 +2723,13 @@
         <v>197</v>
       </c>
       <c r="V18" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W18" s="4"/>
-    </row>
-    <row r="19" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>228</v>
       </c>
@@ -2624,16 +2787,18 @@
       <c r="S19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T19" s="4"/>
+      <c r="T19"/>
       <c r="U19" s="3" t="s">
         <v>205</v>
       </c>
       <c r="V19" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W19" s="4"/>
-    </row>
-    <row r="20" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>229</v>
       </c>
@@ -2694,13 +2859,15 @@
       <c r="T20" s="1">
         <v>9764851329</v>
       </c>
-      <c r="U20" s="4"/>
+      <c r="U20"/>
       <c r="V20" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W20" s="4"/>
-    </row>
-    <row r="21" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row ht="45" r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>230</v>
       </c>
@@ -2765,11 +2932,13 @@
         <v>213</v>
       </c>
       <c r="V21" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W21" s="4"/>
-    </row>
-    <row r="22" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>232</v>
       </c>
@@ -2834,11 +3003,13 @@
         <v>197</v>
       </c>
       <c r="V22" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W22" s="4"/>
-    </row>
-    <row r="23" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W22" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>243</v>
       </c>
@@ -2903,11 +3074,13 @@
         <v>213</v>
       </c>
       <c r="V23" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W23" s="4"/>
-    </row>
-    <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>234</v>
       </c>
@@ -2965,16 +3138,18 @@
       <c r="S24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T24" s="4"/>
+      <c r="T24"/>
       <c r="U24" s="3" t="s">
         <v>205</v>
       </c>
       <c r="V24" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W24" s="4"/>
-    </row>
-    <row r="25" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>237</v>
       </c>
@@ -3029,7 +3204,7 @@
       <c r="R25" s="1">
         <v>975351</v>
       </c>
-      <c r="S25" s="4"/>
+      <c r="S25"/>
       <c r="T25" s="1">
         <v>9756842138</v>
       </c>
@@ -3037,11 +3212,13 @@
         <v>197</v>
       </c>
       <c r="V25" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W25" s="4"/>
-    </row>
-    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W25" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="30" r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>239</v>
       </c>
@@ -3106,11 +3283,13 @@
         <v>113</v>
       </c>
       <c r="V26" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W26" s="4"/>
-    </row>
-    <row r="27" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="60" r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>241</v>
       </c>
@@ -3175,11 +3354,13 @@
         <v>78</v>
       </c>
       <c r="V27" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W27" s="4"/>
-    </row>
-    <row r="28" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="60" r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>242</v>
       </c>
@@ -3244,11 +3425,13 @@
         <v>161</v>
       </c>
       <c r="V28" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W28" s="4"/>
-    </row>
-    <row r="29" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>245</v>
       </c>
@@ -3313,11 +3496,13 @@
         <v>213</v>
       </c>
       <c r="V29" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W29" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>247</v>
       </c>
@@ -3382,11 +3567,13 @@
         <v>213</v>
       </c>
       <c r="V30" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W30" s="4"/>
-    </row>
-    <row r="31" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W30" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>249</v>
       </c>
@@ -3451,11 +3638,13 @@
         <v>143</v>
       </c>
       <c r="V31" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>250</v>
       </c>
@@ -3520,11 +3709,13 @@
         <v>143</v>
       </c>
       <c r="V32" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W32" s="4"/>
-    </row>
-    <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="W32" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row ht="45" r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>251</v>
       </c>
@@ -3589,159 +3780,716 @@
         <v>143</v>
       </c>
       <c r="V33" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="W33" s="4"/>
+        <v>258</v>
+      </c>
+      <c r="W33" t="s">
+        <v>267</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1" xr:uid="{AD2E7342-13F3-4F9E-8E52-A4A5C93E59C5}"/>
-    <hyperlink ref="U3" r:id="rId2" xr:uid="{29E24696-ABE1-400D-9555-90AA7E0B37DB}"/>
-    <hyperlink ref="U4" r:id="rId3" xr:uid="{CCAF1C57-5CAA-46A4-9FDE-DC7CCCBA1FE2}"/>
-    <hyperlink ref="U5" r:id="rId4" xr:uid="{B3D432BD-5DC1-4DC7-8345-27CBF5E7A7B8}"/>
-    <hyperlink ref="U6" r:id="rId5" xr:uid="{3FDA59A3-9F97-476D-940E-F9F8F3419590}"/>
-    <hyperlink ref="U7" r:id="rId6" xr:uid="{EE21543B-4101-44AC-A791-BB020D67D15A}"/>
-    <hyperlink ref="U8" r:id="rId7" xr:uid="{32FDA270-E1F7-4995-8E37-B67AC9DD3235}"/>
-    <hyperlink ref="U9" r:id="rId8" xr:uid="{BF6141EC-4057-4024-874D-477765760585}"/>
-    <hyperlink ref="U10" r:id="rId9" xr:uid="{499AE279-0ED2-4CD7-8F13-139FE1A622CC}"/>
-    <hyperlink ref="U11" r:id="rId10" xr:uid="{3662C424-4C41-4250-B209-CDBACC7A71DA}"/>
-    <hyperlink ref="U12" r:id="rId11" xr:uid="{289EC856-9D51-4814-A650-D5A3B00ECC0C}"/>
-    <hyperlink ref="U13" r:id="rId12" xr:uid="{3457B279-724D-4979-BED6-2B8D01AC0924}"/>
-    <hyperlink ref="U14" r:id="rId13" xr:uid="{BE633FB0-EF01-48CB-8C71-635435699C5D}"/>
-    <hyperlink ref="U15" r:id="rId14" xr:uid="{5A83CB1D-4B01-46C3-8AE1-B39AA1430B94}"/>
-    <hyperlink ref="U16" r:id="rId15" xr:uid="{B14B822F-C21C-45A6-9F7E-B221B6998A4F}"/>
-    <hyperlink ref="U17" r:id="rId16" xr:uid="{17A344FC-B915-4271-BD66-3CE2516C36C9}"/>
-    <hyperlink ref="U18" r:id="rId17" xr:uid="{3F2C047A-5A19-46D7-AC7D-025B60279EC0}"/>
-    <hyperlink ref="U19" r:id="rId18" xr:uid="{9D0F7785-F305-41DD-9E52-2BE70A95E805}"/>
-    <hyperlink ref="U21" r:id="rId19" xr:uid="{87FE59FB-6A12-4CF9-A01C-E45985D7BEB9}"/>
-    <hyperlink ref="U22" r:id="rId20" xr:uid="{94815C58-70FB-4B56-9A95-4C6DF393AB8B}"/>
-    <hyperlink ref="U24" r:id="rId21" xr:uid="{0D5D67AA-0F64-4B48-B39E-51AE702FA16C}"/>
-    <hyperlink ref="U25" r:id="rId22" xr:uid="{96A0CE36-EDF9-4C31-9319-B656541D8E0C}"/>
-    <hyperlink ref="U26" r:id="rId23" xr:uid="{623CADAB-4274-4755-A141-B35BDB09B4B6}"/>
-    <hyperlink ref="U27" r:id="rId24" xr:uid="{B44FE402-C265-4AEF-9B14-D15BF35C1DBA}"/>
-    <hyperlink ref="U28" r:id="rId25" xr:uid="{6512C6AF-E70C-4FF2-9970-5C6D37EB2E59}"/>
-    <hyperlink ref="U23" r:id="rId26" xr:uid="{EFDCE50D-AE7D-4C63-BB97-0273A329B531}"/>
-    <hyperlink ref="U29" r:id="rId27" xr:uid="{5E27030D-F479-497D-9434-F5E7113CE60E}"/>
-    <hyperlink ref="U30" r:id="rId28" xr:uid="{B93A6E59-B895-40DD-BE44-873C07EC1794}"/>
-    <hyperlink ref="U31" r:id="rId29" xr:uid="{CC221388-8D4E-4326-ADBC-A8DF4471F271}"/>
-    <hyperlink ref="U32" r:id="rId30" xr:uid="{8D7E4050-6D3E-4A7F-A832-EDC7FD964D79}"/>
-    <hyperlink ref="U33" r:id="rId31" xr:uid="{CF689C5F-9073-4A89-8BDA-2602AD6EED14}"/>
+    <hyperlink r:id="rId1" ref="U2" xr:uid="{AD2E7342-13F3-4F9E-8E52-A4A5C93E59C5}"/>
+    <hyperlink r:id="rId2" ref="U3" xr:uid="{29E24696-ABE1-400D-9555-90AA7E0B37DB}"/>
+    <hyperlink r:id="rId3" ref="U4" xr:uid="{CCAF1C57-5CAA-46A4-9FDE-DC7CCCBA1FE2}"/>
+    <hyperlink r:id="rId4" ref="U5" xr:uid="{B3D432BD-5DC1-4DC7-8345-27CBF5E7A7B8}"/>
+    <hyperlink r:id="rId5" ref="U6" xr:uid="{3FDA59A3-9F97-476D-940E-F9F8F3419590}"/>
+    <hyperlink r:id="rId6" ref="U7" xr:uid="{EE21543B-4101-44AC-A791-BB020D67D15A}"/>
+    <hyperlink r:id="rId7" ref="U8" xr:uid="{32FDA270-E1F7-4995-8E37-B67AC9DD3235}"/>
+    <hyperlink r:id="rId8" ref="U9" xr:uid="{BF6141EC-4057-4024-874D-477765760585}"/>
+    <hyperlink r:id="rId9" ref="U10" xr:uid="{499AE279-0ED2-4CD7-8F13-139FE1A622CC}"/>
+    <hyperlink r:id="rId10" ref="U11" xr:uid="{3662C424-4C41-4250-B209-CDBACC7A71DA}"/>
+    <hyperlink r:id="rId11" ref="U12" xr:uid="{289EC856-9D51-4814-A650-D5A3B00ECC0C}"/>
+    <hyperlink r:id="rId12" ref="U13" xr:uid="{3457B279-724D-4979-BED6-2B8D01AC0924}"/>
+    <hyperlink r:id="rId13" ref="U14" xr:uid="{BE633FB0-EF01-48CB-8C71-635435699C5D}"/>
+    <hyperlink r:id="rId14" ref="U15" xr:uid="{5A83CB1D-4B01-46C3-8AE1-B39AA1430B94}"/>
+    <hyperlink r:id="rId15" ref="U16" xr:uid="{B14B822F-C21C-45A6-9F7E-B221B6998A4F}"/>
+    <hyperlink r:id="rId16" ref="U17" xr:uid="{17A344FC-B915-4271-BD66-3CE2516C36C9}"/>
+    <hyperlink r:id="rId17" ref="U18" xr:uid="{3F2C047A-5A19-46D7-AC7D-025B60279EC0}"/>
+    <hyperlink r:id="rId18" ref="U19" xr:uid="{9D0F7785-F305-41DD-9E52-2BE70A95E805}"/>
+    <hyperlink r:id="rId19" ref="U21" xr:uid="{87FE59FB-6A12-4CF9-A01C-E45985D7BEB9}"/>
+    <hyperlink r:id="rId20" ref="U22" xr:uid="{94815C58-70FB-4B56-9A95-4C6DF393AB8B}"/>
+    <hyperlink r:id="rId21" ref="U24" xr:uid="{0D5D67AA-0F64-4B48-B39E-51AE702FA16C}"/>
+    <hyperlink r:id="rId22" ref="U25" xr:uid="{96A0CE36-EDF9-4C31-9319-B656541D8E0C}"/>
+    <hyperlink r:id="rId23" ref="U26" xr:uid="{623CADAB-4274-4755-A141-B35BDB09B4B6}"/>
+    <hyperlink r:id="rId24" ref="U27" xr:uid="{B44FE402-C265-4AEF-9B14-D15BF35C1DBA}"/>
+    <hyperlink r:id="rId25" ref="U28" xr:uid="{6512C6AF-E70C-4FF2-9970-5C6D37EB2E59}"/>
+    <hyperlink r:id="rId26" ref="U23" xr:uid="{EFDCE50D-AE7D-4C63-BB97-0273A329B531}"/>
+    <hyperlink r:id="rId27" ref="U29" xr:uid="{5E27030D-F479-497D-9434-F5E7113CE60E}"/>
+    <hyperlink r:id="rId28" ref="U30" xr:uid="{B93A6E59-B895-40DD-BE44-873C07EC1794}"/>
+    <hyperlink r:id="rId29" ref="U31" xr:uid="{CC221388-8D4E-4326-ADBC-A8DF4471F271}"/>
+    <hyperlink r:id="rId30" ref="U32" xr:uid="{8D7E4050-6D3E-4A7F-A832-EDC7FD964D79}"/>
+    <hyperlink r:id="rId31" ref="U33" xr:uid="{CF689C5F-9073-4A89-8BDA-2602AD6EED14}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F6B53-E569-4B89-A652-F5C31A5C1A46}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F6B53-E569-4B89-A652-F5C31A5C1A46}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:M11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4155C7C4-4755-4B58-B329-E8D997F9A4D5}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="A5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8" t="s">
         <v>267</v>
       </c>
-      <c r="D7" s="4" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E489C3-898E-4475-9329-40E4F4E25B0C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27533668-FE42-4807-A074-05720A6BA6EA}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>256</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51642CA-314A-4C79-A936-A52A4B34D23B}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="13">
+        <v>846525493475</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="13">
+        <v>674768648</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49989E7-0313-4F5F-A8E3-2527E248990B}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B575084E-A744-44DE-8C03-634B219836EC}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>